<commit_message>
02.11.2024 - Wyliczenia dla magazynu wydają się zakończone. Czas na raporty.
</commit_message>
<xml_diff>
--- a/bledy/obcokrajowcy.xlsx
+++ b/bledy/obcokrajowcy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjektyPython\place_v2\bledy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD6724E0-03BD-4649-A932-341EE81153E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E65C668-E12A-4A80-95F3-200EC0325761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{E7BA9170-FD15-4C8C-B842-9F866A156A91}"/>
+    <workbookView xWindow="-28650" yWindow="870" windowWidth="28650" windowHeight="14220" xr2:uid="{E7BA9170-FD15-4C8C-B842-9F866A156A91}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>CHARISA SIANA</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>dni w pracy</t>
+  </si>
+  <si>
+    <t>FIKRI MUHAMMAD RIZAL</t>
   </si>
 </sst>
 </file>
@@ -456,10 +459,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D29EA91-5F1A-45A4-ADB6-8EDDBEF07A11}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -623,6 +626,17 @@
         <v>21</v>
       </c>
     </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>6025</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>